<commit_message>
docs: :notebook: update docs
</commit_message>
<xml_diff>
--- a/out/2023-01-14_cb_list.xlsx
+++ b/out/2023-01-14_cb_list.xlsx
@@ -3,33 +3,183 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowHeight="15560" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="All" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="到期保底" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="到期保本" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="回售摸彩" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="低价格低溢价" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="23">
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -39,15 +189,201 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -71,26 +407,316 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -443,7 +1069,6 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -68760,7 +69385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AH5"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -69201,66 +69826,66 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1SoM2PuzSv0UT7LcxkeA7w%3D%3D</t>
+          <t>kcwnSJB8%2BBaQMXTxNDNrCQ%3D%3D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>123107</t>
+          <t>113647</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>温氏转债</t>
+          <t>禾丰转债</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>300498</t>
+          <t>603609</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>温氏股份</t>
+          <t>禾丰股份</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>sz</t>
+          <t>sh</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>127.79</v>
+        <v>127.031</v>
       </c>
       <c r="I4" t="n">
-        <v>1.01</v>
+        <v>0.74</v>
       </c>
       <c r="J4" t="n">
-        <v>20.31</v>
+        <v>12.2</v>
       </c>
       <c r="K4" t="n">
-        <v>3.78</v>
+        <v>1.75</v>
       </c>
       <c r="L4" t="n">
-        <v>1.39</v>
+        <v>0.42</v>
       </c>
       <c r="M4" t="n">
-        <v>17.37</v>
+        <v>10.26</v>
       </c>
       <c r="N4" t="n">
-        <v>9.300000000000001</v>
+        <v>6.8</v>
       </c>
       <c r="O4" t="n">
-        <v>3.77</v>
+        <v>1.64</v>
       </c>
       <c r="P4" t="n">
-        <v>3.23</v>
+        <v>1.38</v>
       </c>
       <c r="Q4" t="n">
-        <v>112.8</v>
+        <v>117.1</v>
       </c>
       <c r="R4" t="n">
-        <v>110.24</v>
+        <v>113.68</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -69269,7 +69894,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>2021-04-21</t>
+          <t>2022-05-18</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
@@ -69279,43 +69904,43 @@
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>4.20年</t>
+          <t>5.27年</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>2.20年</t>
+          <t>3.27年</t>
         </is>
       </c>
       <c r="X4" t="n">
-        <v>77.3867</v>
+        <v>14.67040288</v>
       </c>
       <c r="Y4" t="n">
-        <v>1331</v>
+        <v>112</v>
       </c>
       <c r="Z4" t="n">
-        <v>5.8</v>
+        <v>13.1</v>
       </c>
       <c r="AA4" t="n">
-        <v>-2.98</v>
+        <v>-1.56</v>
       </c>
       <c r="AB4" t="n">
-        <v>-3.51</v>
+        <v>-2.12</v>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>-8.89</t>
+          <t>-5.99</t>
         </is>
       </c>
       <c r="AD4" t="n">
-        <v>138.7</v>
+        <v>135.2</v>
       </c>
       <c r="AE4" t="n">
-        <v>41.2</v>
+        <v>41.3</v>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>AA</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
@@ -69325,7 +69950,7 @@
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>2021-05-10已满足下修条件，且满足下修条件后，超过一个月未公告是否行使下修权利！</t>
+          <t>2022-05-19已满足下修条件，且满足下修条件后，超过一个月未公告是否行使下修权利！</t>
         </is>
       </c>
     </row>
@@ -69335,129 +69960,523 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>nXOlsGOB7MOzA75OgRGjWw%3D%3D</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>110077</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>洪城转债</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>600461</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>洪城环境</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>sh</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>122.502</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="J5" t="n">
+        <v>6.92</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M5" t="n">
+        <v>6.21</v>
+      </c>
+      <c r="N5" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>112.9</v>
+      </c>
+      <c r="R5" t="n">
+        <v>110.32</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>2020-12-17</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>已到</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>3.85年</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>1.85年</t>
+        </is>
+      </c>
+      <c r="X5" t="n">
+        <v>17.67217268</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>75</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-2.12</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>-2.71</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>-9.01</t>
+        </is>
+      </c>
+      <c r="AD5" t="n">
+        <v>133.6</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>AA+</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Cl9KfiriabGa3PwAMsCC6Q%3D%3D</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>128141</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>旺能转债</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>002034</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>旺能环境</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>sz</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>126.9</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="J6" t="n">
+        <v>18.18</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M6" t="n">
+        <v>15.67</v>
+      </c>
+      <c r="N6" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>114.3</v>
+      </c>
+      <c r="R6" t="n">
+        <v>111.44</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>2021-01-18</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>已到</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>3.92年</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>1.92年</t>
+        </is>
+      </c>
+      <c r="X6" t="n">
+        <v>12.7014</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>78</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>-2.68</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>-3.3</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>-9.86</t>
+        </is>
+      </c>
+      <c r="AD6" t="n">
+        <v>137.8</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>AA</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1SoM2PuzSv0UT7LcxkeA7w%3D%3D</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>123107</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>温氏转债</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>300498</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>温氏股份</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>sz</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>127.79</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="J7" t="n">
+        <v>20.31</v>
+      </c>
+      <c r="K7" t="n">
+        <v>3.78</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M7" t="n">
+        <v>17.37</v>
+      </c>
+      <c r="N7" t="n">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>112.8</v>
+      </c>
+      <c r="R7" t="n">
+        <v>110.24</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>2021-04-21</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>已到</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>4.20年</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>2.20年</t>
+        </is>
+      </c>
+      <c r="X7" t="n">
+        <v>77.3867</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>1331</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-2.98</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>-3.51</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>-8.89</t>
+        </is>
+      </c>
+      <c r="AD7" t="n">
+        <v>138.7</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>41.2</v>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>AAA</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>2021-05-10已满足下修条件，且满足下修条件后，超过一个月未公告是否行使下修权利！</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>71ClBUS9TE1Pq2GOD4gNCg%3D%3D</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>128081</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>海亮转债</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>002203</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>海亮股份</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>sz</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="H8" t="n">
         <v>126.109</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I8" t="n">
         <v>-0.23</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J8" t="n">
         <v>11.79</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K8" t="n">
         <v>-0.08</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L8" t="n">
         <v>0.18</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M8" t="n">
         <v>9.619999999999999</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N8" t="n">
         <v>2.9</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O8" t="n">
         <v>2.01</v>
       </c>
-      <c r="P5" t="n">
+      <c r="P8" t="n">
         <v>1.64</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q8" t="n">
         <v>113.3</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R8" t="n">
         <v>110.64</v>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="T8" t="inlineStr">
         <is>
           <t>2019-12-16</t>
         </is>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U8" t="inlineStr">
         <is>
           <t>已到</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V8" t="inlineStr">
         <is>
           <t>2.85年</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="W8" t="inlineStr">
         <is>
           <t>0.85年</t>
         </is>
       </c>
-      <c r="X5" t="n">
+      <c r="X8" t="n">
         <v>28.3646</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="Y8" t="n">
         <v>234</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="Z8" t="n">
         <v>12.1</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AA8" t="n">
         <v>-3.74</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AB8" t="n">
         <v>-4.54</v>
       </c>
-      <c r="AC5" t="inlineStr">
+      <c r="AC8" t="inlineStr">
         <is>
           <t>-19.2</t>
         </is>
       </c>
-      <c r="AD5" t="n">
+      <c r="AD8" t="n">
         <v>129.7</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AE8" t="n">
         <v>28.2</v>
       </c>
-      <c r="AF5" t="inlineStr">
+      <c r="AF8" t="inlineStr">
         <is>
           <t>AA</t>
         </is>
       </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AG8" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="AH5" t="inlineStr">
+      <c r="AH8" t="inlineStr">
         <is>
           <t>2020-09-14已满足下修条件，且满足下修条件后，超过一个月未公告是否行使下修权利！</t>
         </is>

</xml_diff>